<commit_message>
sut2 doc updates 2
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-Composition-jurisdiction-fetal-death-report.xlsx
+++ b/docs/StructureDefinition-Composition-jurisdiction-fetal-death-report.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-13T11:56:10-05:00</t>
+    <t>2024-02-27T09:44:15-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1810,13 +1810,13 @@
     <t>The obstetric estimate of the infant's gestation in completed weeks based on the birth/delivery attendant's final estimate of gestation which should be determined by all perinatal factors and assessments such as ultrasound, but not the neonatal exam</t>
   </si>
   <si>
-    <t>Composition.section:fetus.entry:methodOfDisposition</t>
-  </si>
-  <si>
-    <t>methodOfDisposition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/bfdr/StructureDefinition/Observation-method-of-disposition)
+    <t>Composition.section:fetus.entry:fetalRemainsDispositionMethod</t>
+  </si>
+  <si>
+    <t>fetalRemainsDispositionMethod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/bfdr/StructureDefinition/Observation-fetal-remains-disposition-method)
 </t>
   </si>
   <si>

</xml_diff>